<commit_message>
Created sql script for database, table and sequence
</commit_message>
<xml_diff>
--- a/e-angona.xlsx
+++ b/e-angona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studies\ITU\S4\Programmation\Python Projects\e-angona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5BFF38E-6E40-4F5D-8AF5-A2C87093F941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF929B-00D5-4F8F-BB6B-510DDF16A09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -730,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -744,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Creating church_group class with its propreties
</commit_message>
<xml_diff>
--- a/e-angona.xlsx
+++ b/e-angona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studies\ITU\S4\Programmation\Python Projects\e-angona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCF929B-00D5-4F8F-BB6B-510DDF16A09B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3C673-DA45-4A2A-ABCC-DAAC95A5CB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E18" sqref="E18:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +791,7 @@
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Creating dynamic generalized CRUD method for each models and string utilities
</commit_message>
<xml_diff>
--- a/e-angona.xlsx
+++ b/e-angona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studies\ITU\S4\Programmation\Python Projects\e-angona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3C673-DA45-4A2A-ABCC-DAAC95A5CB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81861329-437A-4585-B4CD-2FCBC434C99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>Project: e-angona</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>ChurchGroup</t>
-  </si>
-  <si>
-    <t>id, name, firstName, group_id</t>
   </si>
   <si>
     <t>getFund(year, Sunday_id) -&gt; Donation[]</t>
@@ -579,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:E19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +762,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>29</v>
@@ -799,7 +796,7 @@
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -810,7 +807,7 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18">
         <v>15</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E19">
         <v>15</v>
@@ -832,7 +829,7 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E20">
         <v>15</v>
@@ -843,7 +840,7 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E21">
         <v>15</v>
@@ -854,10 +851,10 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
       </c>
       <c r="E22">
         <v>5</v>
@@ -868,7 +865,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>15</v>
@@ -879,7 +876,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E24">
         <v>30</v>
@@ -890,7 +887,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
@@ -904,10 +901,10 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26">
         <v>15</v>
@@ -918,10 +915,10 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" t="s">
         <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>46</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -932,10 +929,10 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
         <v>47</v>
-      </c>
-      <c r="D28" t="s">
-        <v>48</v>
       </c>
       <c r="E28">
         <v>30</v>
@@ -946,7 +943,7 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E29">
         <v>30</v>
@@ -957,7 +954,7 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30">
         <v>30</v>
@@ -968,7 +965,7 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -979,13 +976,13 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" t="s">
         <v>55</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>56</v>
-      </c>
-      <c r="D32" t="s">
-        <v>57</v>
       </c>
       <c r="E32">
         <v>15</v>
@@ -996,10 +993,10 @@
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" t="s">
         <v>58</v>
-      </c>
-      <c r="D33" t="s">
-        <v>59</v>
       </c>
       <c r="E33">
         <v>30</v>
@@ -1010,10 +1007,10 @@
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>59</v>
+      </c>
+      <c r="D34" t="s">
         <v>60</v>
-      </c>
-      <c r="D34" t="s">
-        <v>61</v>
       </c>
       <c r="E34">
         <v>30</v>
@@ -1024,7 +1021,7 @@
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39">
         <f>SUM(E2:E34)</f>
@@ -1033,7 +1030,7 @@
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E40">
         <f>E39/60</f>

</xml_diff>

<commit_message>
creating all models classes
</commit_message>
<xml_diff>
--- a/e-angona.xlsx
+++ b/e-angona.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Studies\ITU\S4\Programmation\Python Projects\e-angona\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81861329-437A-4585-B4CD-2FCBC434C99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA7A01C-2787-4C5A-AC68-6B59627F632A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
   </cols>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -860,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -938,7 +938,7 @@
         <v>30</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -949,7 +949,7 @@
         <v>30</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>30</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -971,7 +971,7 @@
         <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>